<commit_message>
sửa dữ liệu file excel. thêm cột LEVER trong bảng s2,s3
</commit_message>
<xml_diff>
--- a/python/N2_test.xlsx
+++ b/python/N2_test.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2210350\Documents\3tpan\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2210314\Documents\3tpan\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE9541-06E7-4025-AF3D-6DB968379EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E33C0-3EA2-4E37-B7C7-0B608E0C0659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{A004B8D4-D813-45D8-A93E-A9CE629A7F4D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A004B8D4-D813-45D8-A93E-A9CE629A7F4D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="s1" sheetId="1" r:id="rId1"/>
+    <sheet name="s2" sheetId="2" r:id="rId2"/>
+    <sheet name="s3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="312">
   <si>
     <t>LEVER</t>
     <phoneticPr fontId="1"/>
@@ -1215,6 +1215,17 @@
   </si>
   <si>
     <t>こい　</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEVER</t>
+  </si>
+  <si>
+    <t>LEVER</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>N2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1659,9 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D52141-9C59-4347-B8B8-827A19FC6E8A}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2043,297 +2052,373 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9CD655-452A-49B4-99B4-C38AB49257A0}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2345,937 +2430,1075 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E06357-5DB5-448F-A5B1-45C28F7523FC}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>121</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>122</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>124</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>125</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>126</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>127</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>128</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>129</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>130</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>131</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>132</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>133</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>134</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>135</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>136</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>137</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>138</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>139</v>
-      </c>
-      <c r="E6" t="s">
-        <v>140</v>
       </c>
       <c r="F6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
+      <c r="G6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>142</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>143</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>144</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>148</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>149</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>150</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>151</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>152</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>153</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>154</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>155</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>156</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="E10" t="s">
-        <v>159</v>
       </c>
       <c r="F10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="10" t="s">
+      <c r="G10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>163</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>162</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>161</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>160</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>164</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>165</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>166</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>167</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>168</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>169</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>170</v>
-      </c>
-      <c r="E13" t="s">
-        <v>171</v>
       </c>
       <c r="F13" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+      <c r="G13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>172</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>173</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>175</v>
-      </c>
-      <c r="E14" t="s">
-        <v>174</v>
       </c>
       <c r="F14" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="10" t="s">
+      <c r="G14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>176</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>177</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>178</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>179</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>180</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>181</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>182</v>
-      </c>
-      <c r="E16" t="s">
-        <v>183</v>
       </c>
       <c r="F16" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+      <c r="G16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>190</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>191</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>192</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>193</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>194</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>195</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>196</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>197</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>198</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>199</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>200</v>
-      </c>
-      <c r="E19" t="s">
-        <v>201</v>
       </c>
       <c r="F19" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10" t="s">
+      <c r="G19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>202</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>203</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>204</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>205</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>206</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>207</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>208</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>209</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>210</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>211</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>212</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>213</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>214</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>215</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>216</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>217</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>218</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>219</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>220</v>
-      </c>
-      <c r="E24" t="s">
-        <v>221</v>
       </c>
       <c r="F24" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10" t="s">
+      <c r="G24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>222</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>223</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>224</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>225</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>226</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>227</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>228</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>229</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>231</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>232</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>233</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>234</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>235</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>236</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>232</v>
-      </c>
-      <c r="E28" t="s">
-        <v>237</v>
       </c>
       <c r="F28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="9" t="s">
+      <c r="G28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>238</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>239</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>240</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>241</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>242</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>243</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>244</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>245</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>246</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>247</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>248</v>
-      </c>
-      <c r="E31" t="s">
-        <v>249</v>
       </c>
       <c r="F31" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="9" t="s">
+      <c r="G31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>250</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>251</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>252</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>253</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>254</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>255</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>256</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>257</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>258</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>259</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>234</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>260</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>261</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>262</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>255</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>256</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>263</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>252</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>264</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>265</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="11" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>269</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>270</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>271</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>272</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="11" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>273</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>274</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>275</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>276</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="11" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>277</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>278</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>279</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>280</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="11" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>281</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>282</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>283</v>
-      </c>
-      <c r="E40" t="s">
-        <v>284</v>
       </c>
       <c r="F40" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="11" t="s">
+      <c r="G40" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>276</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>285</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>286</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>287</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>288</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>289</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>290</v>
-      </c>
-      <c r="E42" t="s">
-        <v>291</v>
       </c>
       <c r="F42" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="11" t="s">
+      <c r="G42" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>292</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>293</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>294</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>295</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>296</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>297</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>298</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>299</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="11" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>280</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>300</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>301</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>302</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="11" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>303</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>304</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>305</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>306</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>308</v>
       </c>
     </row>

</xml_diff>